<commit_message>
Add 05 11 + mt
</commit_message>
<xml_diff>
--- a/RPL_V2/xlsx/club_krasnodar.xlsx
+++ b/RPL_V2/xlsx/club_krasnodar.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView minimized="1" xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet" sheetId="1" r:id="rId1"/>
@@ -1006,8 +1006,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="G23" sqref="E23:G23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>